<commit_message>
tables added: heating technologies, radiator, building components.
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Scenario_BuildingComponent_Option.xlsx
+++ b/projects/test_building/input/Scenario_BuildingComponent_Option.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEBDB55-A8EC-BE48-A6B5-D4E00923588C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271D996F-B910-8E48-8E8A-5DD14B68E8ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -425,7 +425,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>